<commit_message>
complete MapData & subMap
</commit_message>
<xml_diff>
--- a/src/main/resources/edge.xlsx
+++ b/src/main/resources/edge.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20349"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20350"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8f55eab75a13572/2019-2020-1/数据结构课设/BJUT-Tour-Guide/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbyto\OneDrive\2019-2020-1\数据结构课设\BJUT-Tour-Guide\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="6_{C993092A-A8D6-42DF-BBBA-81197CE1F091}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{ED9299DF-B580-497E-BA16-B0BFFA02B826}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="6_{C993092A-A8D6-42DF-BBBA-81197CE1F091}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F36685B1-D467-45EC-9A74-E94FDEFB6132}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23451" windowHeight="11297" xr2:uid="{528109DF-C4F4-4C5E-9FCD-53E11326FFBA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="105">
   <si>
     <t>0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -260,6 +260,190 @@
   </si>
   <si>
     <t>41</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>67</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>94</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>146</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>87</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>163</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>104</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>109</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>78</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>132</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>97</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>41</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>46</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>113</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>115</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>161</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>76</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>153</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>261</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>54</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -318,15 +502,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -650,17 +831,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06805234-9307-4AFE-BE19-153F90616554}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="5.640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.640625" style="2"/>
+    <col min="1" max="3" width="5.640625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +853,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +865,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -696,7 +877,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -708,7 +889,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -720,7 +901,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -732,7 +913,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -744,7 +925,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -756,7 +937,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -768,7 +949,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -780,7 +961,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -792,7 +973,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -804,7 +985,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -816,19 +997,19 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -840,394 +1021,533 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C18" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C19" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C21" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C22" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C27" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C28" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C29" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C30" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C31" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C32" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C33" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C34" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C37" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C39" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C41" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="1"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="1"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="1"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="1"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="1"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="1"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="1"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="1"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C42" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
     </row>
   </sheetData>

</xml_diff>